<commit_message>
Finished the 1st batch of discoveries
</commit_message>
<xml_diff>
--- a/docs/Metrics.xlsx
+++ b/docs/Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr backupFile="1"/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13095" activeTab="1"/>
+    <workbookView windowWidth="28695" windowHeight="13095"/>
   </bookViews>
   <sheets>
     <sheet name="Discoveries" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332">
   <si>
     <t>Discovery ID</t>
   </si>
@@ -28,148 +28,487 @@
     <t>MacroNames</t>
   </si>
   <si>
+    <t>FQDN</t>
+  </si>
+  <si>
+    <t>Implementation Status</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
     <t>External IPs involved in pinging  the organization in the last week</t>
   </si>
   <si>
     <t>EXT_IP</t>
   </si>
   <si>
+    <t>discover.external_ips_pinging_the_org</t>
+  </si>
+  <si>
     <t>External IPs involved in connections to the organization in the last week</t>
   </si>
   <si>
+    <t>discover.external_ips_connecting_to_the_org</t>
+  </si>
+  <si>
     <t>Organization public IPs involved in connections from the outside in the last week</t>
   </si>
   <si>
     <t>PUB_IP</t>
   </si>
   <si>
+    <t>discover.public_org_ips_connected_to_from_outside_the_org</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>The data currently doesn't have that info</t>
+  </si>
+  <si>
     <t>Organization public IPs involved in connections from the outside in the last week and the list of dest ports used</t>
   </si>
   <si>
     <t>PUB_IP, DPORT</t>
   </si>
   <si>
+    <t>discover.public_org_ips_and_ports_connected_to_from_outside_the_org</t>
+  </si>
+  <si>
     <t>DNS servers in the organization</t>
   </si>
   <si>
     <t>DNS_IP</t>
   </si>
   <si>
+    <t>discover.org_dns_servers</t>
+  </si>
+  <si>
     <t>Top n most frequently queried DNS fqdns</t>
   </si>
   <si>
     <t>DNS_REC</t>
   </si>
   <si>
+    <t>discover.top_n_most_frequently_queried_fqdns</t>
+  </si>
+  <si>
     <t>Top n rarely queried DNS fqdns</t>
   </si>
   <si>
+    <t>discover.top_n_most_rarely_queried_fqdns</t>
+  </si>
+  <si>
     <t>LAN Servers IPs</t>
   </si>
   <si>
     <t>SERVER_IP</t>
   </si>
   <si>
+    <t>discover.lan_servers_ips</t>
+  </si>
+  <si>
     <t>LAN Workstations IPs</t>
   </si>
   <si>
     <t>WORKSTAION_IP</t>
   </si>
   <si>
+    <t>discover.lan_workstation_ips</t>
+  </si>
+  <si>
     <t>Crown jewels IPs</t>
   </si>
   <si>
     <t>CROWN_JEWEL_IP</t>
   </si>
   <si>
+    <t>discover.crown_jewels_ips</t>
+  </si>
+  <si>
     <t>LAN IPs</t>
   </si>
   <si>
     <t>LAN_IP</t>
   </si>
   <si>
+    <t>discover.lan_ips</t>
+  </si>
+  <si>
     <t>DNS query flags</t>
   </si>
   <si>
     <t>DNS_QRY_FLAG</t>
   </si>
   <si>
-    <t>TFTP servers</t>
+    <t>discover.dns_query_flags</t>
+  </si>
+  <si>
+    <t>TFTP servers in the organization</t>
   </si>
   <si>
     <t>TFTP_SRV_IP</t>
   </si>
   <si>
+    <t>discover.org_tftp_servers</t>
+  </si>
+  <si>
     <t>HTTP Methods used per WebServer</t>
   </si>
   <si>
+    <t>VIRT_HOST,HTTP_VERB</t>
+  </si>
+  <si>
+    <t>discover.webservers_webmethods</t>
+  </si>
+  <si>
+    <t>Target ports used to connect to each workstation IP</t>
+  </si>
+  <si>
+    <t>WKSTA_IP,DPORT</t>
+  </si>
+  <si>
+    <t>discover.dst_workstations_dst_ports</t>
+  </si>
+  <si>
+    <t>Target ports used to connect to each &lt;function (sql, web, exchange, ...)&gt; server IP</t>
+  </si>
+  <si>
+    <t>SRVR_IP,DPORT</t>
+  </si>
+  <si>
+    <t>Target ports used to connect to each &lt;function (mail, websites, ...)&gt; DMZ IP</t>
+  </si>
+  <si>
+    <t>DMZ_IP,DPORT</t>
+  </si>
+  <si>
+    <t>Target ports used to connect to each public IP</t>
+  </si>
+  <si>
+    <t>DPORT</t>
+  </si>
+  <si>
+    <t>External IPs involved in connections from the organization in the last week</t>
+  </si>
+  <si>
+    <t>discover.external_ips_connected_to_by_org</t>
+  </si>
+  <si>
+    <t>Issuer of SSL/TLS certificates of websites accessed by the organization's internal IPs in the last week</t>
+  </si>
+  <si>
+    <t>CERT_ISSUER</t>
+  </si>
+  <si>
+    <t>discover.certs_issuers</t>
+  </si>
+  <si>
+    <t>CN of SSL/TLS certificates of websites accessed by the organization's internal IPs in the last week</t>
+  </si>
+  <si>
+    <t>CERT_CN</t>
+  </si>
+  <si>
+    <t>discover.certs_cn</t>
+  </si>
+  <si>
+    <t>Top n most frequently used mail senders (from outside the organization)</t>
+  </si>
+  <si>
+    <t>MAIL_ADDR</t>
+  </si>
+  <si>
+    <t>Top n rarely used mail senders (from outside the organization)</t>
+  </si>
+  <si>
+    <t>Volumes (e.g. C:, D:, E:)</t>
+  </si>
+  <si>
+    <t>VOL</t>
+  </si>
+  <si>
+    <t>Web servers</t>
+  </si>
+  <si>
+    <t>discover.org_web_servers</t>
+  </si>
+  <si>
+    <t>Website pages</t>
+  </si>
+  <si>
+    <t>VIRT_HOST,URL</t>
+  </si>
+  <si>
+    <t>discover.website_pages</t>
+  </si>
+  <si>
+    <t>Website files</t>
+  </si>
+  <si>
+    <t>WEB_FILE</t>
+  </si>
+  <si>
+    <t>discover.website_files</t>
+  </si>
+  <si>
+    <t>Website folders</t>
+  </si>
+  <si>
+    <t>FOLDER_PATH</t>
+  </si>
+  <si>
+    <t>Needs further processing ontop of elastic aggregation</t>
+  </si>
+  <si>
+    <t>Firewall policies</t>
+  </si>
+  <si>
+    <t>FW_RULE_ID</t>
+  </si>
+  <si>
+    <t>Event types</t>
+  </si>
+  <si>
+    <t>EVENT_TYPE</t>
+  </si>
+  <si>
+    <t>discover.types</t>
+  </si>
+  <si>
+    <t>User-agents detected</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>discover.useragents</t>
+  </si>
+  <si>
+    <t>LAN Hostnames</t>
+  </si>
+  <si>
+    <t>HOST</t>
+  </si>
+  <si>
+    <t>Websites (URLs + ports)</t>
+  </si>
+  <si>
+    <t>WEBSITE,WEBPORT</t>
+  </si>
+  <si>
+    <t>discover.websites_ports</t>
+  </si>
+  <si>
+    <t>NAS storage devices</t>
+  </si>
+  <si>
+    <t>NAS_DEV</t>
+  </si>
+  <si>
+    <t>External website virtual host</t>
+  </si>
+  <si>
+    <t>EXT_WEB_VHOST</t>
+  </si>
+  <si>
+    <t>discover.external_website_vhost</t>
+  </si>
+  <si>
+    <t>External website uri</t>
+  </si>
+  <si>
+    <t>EXT_WEB_URI</t>
+  </si>
+  <si>
+    <t>discover.external_website_uri</t>
+  </si>
+  <si>
+    <t>Destination continent</t>
+  </si>
+  <si>
+    <t>EXT_DEST_CONTINENT</t>
+  </si>
+  <si>
+    <t>discover.external_destination_continents_from_org</t>
+  </si>
+  <si>
+    <t>Destination countries</t>
+  </si>
+  <si>
+    <t>EXT_DEST_COUNTRY</t>
+  </si>
+  <si>
+    <t>discover.external_destination_countries_from_org</t>
+  </si>
+  <si>
+    <t>Destination cities</t>
+  </si>
+  <si>
+    <t>EXT_DEST_CITY</t>
+  </si>
+  <si>
+    <t>discover.external_destination_cities_from_org</t>
+  </si>
+  <si>
+    <t>Top n most frequently queried DNS subdomains</t>
+  </si>
+  <si>
+    <t>DNS_SUBDOMAIN</t>
+  </si>
+  <si>
+    <t>discover.top_n_most_frequently_queried_subdomains</t>
+  </si>
+  <si>
+    <t>Top n rarely queried DNS subdomains</t>
+  </si>
+  <si>
+    <t>discover.top_n_most_rarely_queried_subdomains</t>
+  </si>
+  <si>
+    <t>Top n most frequently queried DNS TLDs</t>
+  </si>
+  <si>
+    <t>DNS_TLD</t>
+  </si>
+  <si>
+    <t>discover.top_n_most_frequently_queried_tlds</t>
+  </si>
+  <si>
+    <t>Top n rarely queried DNS TLDs</t>
+  </si>
+  <si>
+    <t>discover.top_n_most_rarely_queried_tlds</t>
+  </si>
+  <si>
+    <t>Top n most frequently queried DNS tld.subdomains</t>
+  </si>
+  <si>
+    <t>DNS_TLD_SUBDOMAIN</t>
+  </si>
+  <si>
+    <t>discover.top_n_most_frequently_queried_tld_subdomains</t>
+  </si>
+  <si>
+    <t>Top n rarely queried DNS tld.subdomains</t>
+  </si>
+  <si>
+    <t>discover.top_n_most_rarely_queried_tld_subdomains</t>
+  </si>
+  <si>
+    <t>Top n most frequently queried DNS query class names</t>
+  </si>
+  <si>
+    <t>DNS_QRY_CLASS</t>
+  </si>
+  <si>
+    <t>discover.top_n_most_frequently_queried_class_names</t>
+  </si>
+  <si>
+    <t>Top n rarely queried DNS query class names</t>
+  </si>
+  <si>
+    <t>discover.top_n_most_rarely_queried_class_names</t>
+  </si>
+  <si>
+    <t>Top n most frequently queried DNS parent domains</t>
+  </si>
+  <si>
+    <t>DNS_PARENT_DOMAIN</t>
+  </si>
+  <si>
+    <t>discover.top_n_most_frequently_queried_parent_domains</t>
+  </si>
+  <si>
+    <t>Top n rarely queried DNS parent domains</t>
+  </si>
+  <si>
+    <t>discover.top_n_most_rarely_queried_parent_domains</t>
+  </si>
+  <si>
+    <t>DNS servers outside the organization</t>
+  </si>
+  <si>
+    <t>discover.external_dns_servers</t>
+  </si>
+  <si>
+    <t>FTP servers in the organization</t>
+  </si>
+  <si>
+    <t>FTP_SERVER</t>
+  </si>
+  <si>
+    <t>discover.org_ftp_servers</t>
+  </si>
+  <si>
+    <t>MS SQL servers in the organization</t>
+  </si>
+  <si>
+    <t>MSSQL_SERVER</t>
+  </si>
+  <si>
+    <t>discover.org_mssql_servers</t>
+  </si>
+  <si>
+    <t>MySQL servers in the organization</t>
+  </si>
+  <si>
+    <t>MYSQL_SERVER</t>
+  </si>
+  <si>
+    <t>discover.org_mysql_servers</t>
+  </si>
+  <si>
+    <t>PostgreSQL servers in the organization</t>
+  </si>
+  <si>
+    <t>PGSQL_SERVER</t>
+  </si>
+  <si>
+    <t>discover.org_pgsql_servers</t>
+  </si>
+  <si>
+    <t>LDAP servers in the organization</t>
+  </si>
+  <si>
+    <t>LDAP_SERVER</t>
+  </si>
+  <si>
+    <t>discover.org_ldap_servers</t>
+  </si>
+  <si>
+    <t>DHCP servers in the organization</t>
+  </si>
+  <si>
+    <t>DHCP_SERVER</t>
+  </si>
+  <si>
+    <t>discover.org_dhcp_servers</t>
+  </si>
+  <si>
+    <t>SSH servers in the organization</t>
+  </si>
+  <si>
+    <t>SSH_SERVER</t>
+  </si>
+  <si>
+    <t>discover.org_ssh_servers</t>
+  </si>
+  <si>
+    <t>HTTP WebMethods used for servers in the org</t>
+  </si>
+  <si>
     <t>HTTP_VERB</t>
   </si>
   <si>
-    <t>Target ports used to connect to each workstation IP</t>
-  </si>
-  <si>
-    <t>DPORT</t>
-  </si>
-  <si>
-    <t>Target ports used to connect to each &lt;function (sql, web, exchange, ...)&gt; server IP</t>
-  </si>
-  <si>
-    <t>Target ports used to connect to each &lt;function (mail, websites, ...)&gt; DMZ IP</t>
-  </si>
-  <si>
-    <t>Target ports used to connect to each public IP</t>
-  </si>
-  <si>
-    <t>External IPs involved in connections from the organization in the last week</t>
-  </si>
-  <si>
-    <t>Issuer of SSL/TLS certificates of websites accessed by the organization's internal IPs in the last week</t>
-  </si>
-  <si>
-    <t>CERT_ISSUER</t>
-  </si>
-  <si>
-    <t>CN of SSL/TLS certificates of websites accessed by the organization's internal IPs in the last week</t>
-  </si>
-  <si>
-    <t>CERT_CN</t>
-  </si>
-  <si>
-    <t>Top n most frequently used mail senders (from outside the organization)</t>
-  </si>
-  <si>
-    <t>MAIL_ADDR</t>
-  </si>
-  <si>
-    <t>Top n rarely used mail senders (from outside the organization)</t>
-  </si>
-  <si>
-    <t>Volumes (e.g. C:, D:, E:)</t>
-  </si>
-  <si>
-    <t>VOL</t>
-  </si>
-  <si>
-    <t>Web servers</t>
-  </si>
-  <si>
-    <t>Website pages</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Website files</t>
-  </si>
-  <si>
-    <t>WEB_FILE</t>
-  </si>
-  <si>
-    <t>Website folders</t>
-  </si>
-  <si>
-    <t>FOLDER_PATH</t>
+    <t>discover.org_http_verbs</t>
+  </si>
+  <si>
+    <t>HTTP WebMethods used for servers outside the org</t>
+  </si>
+  <si>
+    <t>discover.ext_http_verbs</t>
   </si>
   <si>
     <t>Metric</t>
@@ -178,7 +517,7 @@
     <t>Family</t>
   </si>
   <si>
-    <t>FQDN</t>
+    <t>Current uri in sampler</t>
   </si>
   <si>
     <t>Number of pings from EXT_IP to DMZs or LAN IPs</t>
@@ -479,6 +818,177 @@
   </si>
   <si>
     <t>smart-onion.metrics.lateral_movement.number_of_smbv1_connections_to_crown_jewl.xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>Number of __grokparsefailure errors in the last 10 mins</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.health.number_of_grokparsefailures</t>
+  </si>
+  <si>
+    <t>grokparsefailure_count</t>
+  </si>
+  <si>
+    <t>Number of windows events on host</t>
+  </si>
+  <si>
+    <t>WierdBehaviour</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.generally_suspicious.number_of_windows_events_on_host.xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>count_events_on_host</t>
+  </si>
+  <si>
+    <t>Number of IDS alerts on host</t>
+  </si>
+  <si>
+    <t>IDS</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.ids.number_of_ids_alerts_on_host.xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>ids_alerts_for_host</t>
+  </si>
+  <si>
+    <t>Number of IDS attacks on host</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.ids.number_of_ids_attacks_on_host.xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>ids_attacks_for_host</t>
+  </si>
+  <si>
+    <t>Drops per organization's public IP (as destination)</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.reconnaissance.drops_per_org_public_dst_ip.xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>drops_per_internal_dstip</t>
+  </si>
+  <si>
+    <t>Drops per organization's internal IP (as source)</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.c2.drops_per_org_internal_src_ip.xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>drops_per_internal_srcip</t>
+  </si>
+  <si>
+    <t>Drops per FW_RULE_ID</t>
+  </si>
+  <si>
+    <t>HumanError</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.human_error.drops_per_fw_policy_id.xxxx</t>
+  </si>
+  <si>
+    <t>number_of_drops_per_policy</t>
+  </si>
+  <si>
+    <t>Number of events per type</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.health.number_of_events_per_type.ttttt</t>
+  </si>
+  <si>
+    <t>events_per_type</t>
+  </si>
+  <si>
+    <t>Number of events per source LAN_IP</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.health.number_of_events_per_src_ip.xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>events_per_source_ip</t>
+  </si>
+  <si>
+    <t>Number of events per source EXT_IP</t>
+  </si>
+  <si>
+    <t>Number of events per destination LAN_IP</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.health.number_of_events_per_dst_ip.xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>events_per_destination_ip</t>
+  </si>
+  <si>
+    <t>Number of events per destination EXT_IP</t>
+  </si>
+  <si>
+    <t>Number of events per UA</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.health.number_of_events_per_user_agent.aaaaa</t>
+  </si>
+  <si>
+    <t>events_per_useragent</t>
+  </si>
+  <si>
+    <t>Number of handle manipulations and audit events per HOST</t>
+  </si>
+  <si>
+    <t>Host Behaviour</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.host_behaviour.number_of_handle_manipulation_and_audit_events_per_host.aaaaaaa</t>
+  </si>
+  <si>
+    <t>number_of_handle_manipulation_and_audit_events_per_host</t>
+  </si>
+  <si>
+    <t>Number of IIS logged events per host+port (WEBSITE,WEBPORT)</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.host_behaviour.number_of_iis_events_per_site.xxx.xxx.xxx.xxx.nnnn</t>
+  </si>
+  <si>
+    <t>number_of_iis_log_reports_for_host_on_port</t>
+  </si>
+  <si>
+    <t>Number of eicar virus alerts per NAS device (NAS_DEV)</t>
+  </si>
+  <si>
+    <t>SecurityHealth</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.security_health.number_of_eicar_virus_alerts_per_storage_device.xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>number_of_eicar_test_file</t>
+  </si>
+  <si>
+    <t>Number of IIS logged events per webserver (SERVER_IP)</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.host_behaviour.number_of_iis_events_per_server.xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>number_of_iis_log_reports</t>
+  </si>
+  <si>
+    <t>Number of events per day</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.health.number_of_events_per_day</t>
+  </si>
+  <si>
+    <t>events_per_day</t>
   </si>
   <si>
     <t>Workstations</t>
@@ -510,18 +1020,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.3"/>
+      <color rgb="FF660E7A"/>
+      <name val="DejaVu Sans Mono"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -531,8 +1048,85 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -554,34 +1148,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -593,52 +1163,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -660,16 +1185,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -684,7 +1201,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -696,7 +1285,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -708,25 +1321,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -738,133 +1381,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -878,17 +1395,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -912,7 +1438,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -928,26 +1454,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -966,174 +1492,183 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1450,20 +1985,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="12.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="100.428571428571" customWidth="1"/>
-    <col min="3" max="3" width="18.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="22.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="73.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="23.2857142857143" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1473,412 +2010,1153 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>52</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>54</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>56</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>66</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>66</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>69</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>76</v>
+      </c>
+      <c r="D28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
+        <v>79</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E40" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" t="s">
+        <v>120</v>
+      </c>
+      <c r="E44" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>47</v>
       </c>
+      <c r="B48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" t="s">
+        <v>130</v>
+      </c>
+      <c r="E48" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" t="s">
+        <v>132</v>
+      </c>
+      <c r="D49" t="s">
+        <v>133</v>
+      </c>
+      <c r="E49" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" t="s">
+        <v>135</v>
+      </c>
+      <c r="E50" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" t="s">
+        <v>137</v>
+      </c>
+      <c r="E51" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" t="s">
+        <v>139</v>
+      </c>
+      <c r="D52" t="s">
+        <v>140</v>
+      </c>
+      <c r="E52" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" t="s">
+        <v>142</v>
+      </c>
+      <c r="D53" t="s">
+        <v>143</v>
+      </c>
+      <c r="E53" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" t="s">
+        <v>146</v>
+      </c>
+      <c r="E54" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>150</v>
+      </c>
+      <c r="C56" t="s">
+        <v>151</v>
+      </c>
+      <c r="D56" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>153</v>
+      </c>
+      <c r="C57" t="s">
+        <v>154</v>
+      </c>
+      <c r="D57" t="s">
+        <v>155</v>
+      </c>
+      <c r="E57" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>156</v>
+      </c>
+      <c r="C58" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58" t="s">
+        <v>158</v>
+      </c>
+      <c r="E58" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>159</v>
+      </c>
+      <c r="C59" t="s">
+        <v>160</v>
+      </c>
+      <c r="D59" t="s">
+        <v>161</v>
+      </c>
+      <c r="E59" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>162</v>
+      </c>
+      <c r="C60" t="s">
+        <v>160</v>
+      </c>
+      <c r="D60" t="s">
+        <v>163</v>
+      </c>
+      <c r="E60" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1886,32 +3164,36 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="12.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="132.428571428571" customWidth="1"/>
     <col min="3" max="3" width="53.7142857142857" customWidth="1"/>
     <col min="4" max="4" width="108.571428571429" customWidth="1"/>
+    <col min="5" max="5" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>164</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1919,13 +3201,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1933,13 +3215,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>171</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1947,13 +3229,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1961,13 +3243,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1975,13 +3257,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>179</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>180</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1989,13 +3271,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>180</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2003,13 +3285,13 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>168</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2017,13 +3299,13 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>180</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2031,13 +3313,13 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>180</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2045,13 +3327,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>189</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2059,13 +3341,13 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>190</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>191</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2073,13 +3355,13 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>193</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>194</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2087,13 +3369,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2101,13 +3383,13 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>198</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>199</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2115,13 +3397,13 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>201</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>199</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2129,13 +3411,13 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>203</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>204</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2143,13 +3425,13 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>93</v>
+        <v>206</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>207</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2157,13 +3439,13 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>210</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2171,13 +3453,13 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>213</v>
       </c>
       <c r="D20" t="s">
-        <v>101</v>
+        <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2185,13 +3467,13 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>213</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2199,13 +3481,13 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>213</v>
       </c>
       <c r="D22" t="s">
-        <v>101</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2213,13 +3495,13 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>212</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>213</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2227,13 +3509,13 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>102</v>
+        <v>215</v>
       </c>
       <c r="C24" t="s">
-        <v>103</v>
+        <v>216</v>
       </c>
       <c r="D24" t="s">
-        <v>104</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2241,13 +3523,13 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>218</v>
       </c>
       <c r="C25" t="s">
-        <v>103</v>
+        <v>216</v>
       </c>
       <c r="D25" t="s">
-        <v>104</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2255,13 +3537,13 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>219</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>216</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2269,13 +3551,13 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>220</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>221</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2283,13 +3565,13 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>223</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>224</v>
       </c>
       <c r="D28" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2297,13 +3579,13 @@
         <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>226</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>227</v>
       </c>
       <c r="D29" t="s">
-        <v>115</v>
+        <v>228</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2311,13 +3593,13 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>229</v>
       </c>
       <c r="C30" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="D30" t="s">
-        <v>118</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2325,13 +3607,13 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>232</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="D31" t="s">
-        <v>120</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2339,13 +3621,13 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>234</v>
       </c>
       <c r="C32" t="s">
-        <v>122</v>
+        <v>235</v>
       </c>
       <c r="D32" t="s">
-        <v>123</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2353,13 +3635,13 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="C33" t="s">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="D33" t="s">
-        <v>126</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2367,13 +3649,13 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>234</v>
       </c>
       <c r="C34" t="s">
-        <v>122</v>
+        <v>235</v>
       </c>
       <c r="D34" t="s">
-        <v>123</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2381,13 +3663,13 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>127</v>
+        <v>240</v>
       </c>
       <c r="C35" t="s">
-        <v>128</v>
+        <v>241</v>
       </c>
       <c r="D35" t="s">
-        <v>129</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2395,13 +3677,13 @@
         <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>130</v>
+        <v>243</v>
       </c>
       <c r="C36" t="s">
-        <v>128</v>
+        <v>241</v>
       </c>
       <c r="D36" t="s">
-        <v>131</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2409,13 +3691,13 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>245</v>
       </c>
       <c r="C37" t="s">
-        <v>128</v>
+        <v>241</v>
       </c>
       <c r="D37" t="s">
-        <v>133</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2423,13 +3705,13 @@
         <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>134</v>
+        <v>247</v>
       </c>
       <c r="C38" t="s">
-        <v>135</v>
+        <v>248</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2437,13 +3719,13 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>137</v>
+        <v>250</v>
       </c>
       <c r="C39" t="s">
-        <v>138</v>
+        <v>251</v>
       </c>
       <c r="D39" t="s">
-        <v>139</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2451,13 +3733,13 @@
         <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>140</v>
+        <v>253</v>
       </c>
       <c r="C40" t="s">
-        <v>141</v>
+        <v>254</v>
       </c>
       <c r="D40" t="s">
-        <v>142</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2465,70 +3747,380 @@
         <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>256</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>254</v>
       </c>
       <c r="D41" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>0</v>
+      </c>
       <c r="B42" t="s">
-        <v>145</v>
+        <v>258</v>
       </c>
       <c r="C42" t="s">
-        <v>146</v>
+        <v>259</v>
       </c>
       <c r="D42" t="s">
-        <v>147</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="2">
+      <c r="A43">
         <v>8</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>148</v>
+      <c r="B43" t="s">
+        <v>261</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>224</v>
       </c>
       <c r="D43" t="s">
-        <v>149</v>
+        <v>262</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="2">
+      <c r="A44">
         <v>9</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>150</v>
+      <c r="B44" t="s">
+        <v>263</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>151</v>
+        <v>224</v>
+      </c>
+      <c r="D44" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="2">
+      <c r="A45">
         <v>10</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>152</v>
+      <c r="B45" t="s">
+        <v>265</v>
       </c>
       <c r="C45" t="s">
-        <v>111</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>153</v>
+        <v>224</v>
+      </c>
+      <c r="D45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>267</v>
+      </c>
+      <c r="C46" t="s">
+        <v>268</v>
+      </c>
+      <c r="D46" t="s">
+        <v>269</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>271</v>
+      </c>
+      <c r="C47" t="s">
+        <v>272</v>
+      </c>
+      <c r="D47" t="s">
+        <v>273</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>11</v>
+      </c>
+      <c r="B48" t="s">
+        <v>275</v>
+      </c>
+      <c r="C48" t="s">
+        <v>276</v>
+      </c>
+      <c r="D48" t="s">
+        <v>277</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>279</v>
+      </c>
+      <c r="C49" t="s">
+        <v>276</v>
+      </c>
+      <c r="D49" t="s">
+        <v>280</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>282</v>
+      </c>
+      <c r="C50" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" t="s">
+        <v>283</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>11</v>
+      </c>
+      <c r="B51" t="s">
+        <v>285</v>
+      </c>
+      <c r="C51" t="s">
+        <v>286</v>
+      </c>
+      <c r="D51" t="s">
+        <v>287</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>29</v>
+      </c>
+      <c r="B52" t="s">
+        <v>289</v>
+      </c>
+      <c r="C52" t="s">
+        <v>290</v>
+      </c>
+      <c r="D52" t="s">
+        <v>291</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>30</v>
+      </c>
+      <c r="B53" t="s">
+        <v>293</v>
+      </c>
+      <c r="C53" t="s">
+        <v>268</v>
+      </c>
+      <c r="D53" t="s">
+        <v>294</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>11</v>
+      </c>
+      <c r="B54" t="s">
+        <v>296</v>
+      </c>
+      <c r="C54" t="s">
+        <v>268</v>
+      </c>
+      <c r="D54" t="s">
+        <v>297</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>299</v>
+      </c>
+      <c r="C55" t="s">
+        <v>268</v>
+      </c>
+      <c r="D55" t="s">
+        <v>297</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56">
+        <v>11</v>
+      </c>
+      <c r="B56" t="s">
+        <v>300</v>
+      </c>
+      <c r="C56" t="s">
+        <v>268</v>
+      </c>
+      <c r="D56" t="s">
+        <v>301</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57">
+        <v>19</v>
+      </c>
+      <c r="B57" t="s">
+        <v>303</v>
+      </c>
+      <c r="C57" t="s">
+        <v>268</v>
+      </c>
+      <c r="D57" t="s">
+        <v>301</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <v>31</v>
+      </c>
+      <c r="B58" t="s">
+        <v>304</v>
+      </c>
+      <c r="C58" t="s">
+        <v>268</v>
+      </c>
+      <c r="D58" t="s">
+        <v>305</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <v>32</v>
+      </c>
+      <c r="B59" t="s">
+        <v>307</v>
+      </c>
+      <c r="C59" t="s">
+        <v>308</v>
+      </c>
+      <c r="D59" t="s">
+        <v>309</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <v>33</v>
+      </c>
+      <c r="B60" t="s">
+        <v>311</v>
+      </c>
+      <c r="C60" t="s">
+        <v>308</v>
+      </c>
+      <c r="D60" t="s">
+        <v>312</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <v>34</v>
+      </c>
+      <c r="B61" t="s">
+        <v>314</v>
+      </c>
+      <c r="C61" t="s">
+        <v>315</v>
+      </c>
+      <c r="D61" t="s">
+        <v>316</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62">
+        <v>25</v>
+      </c>
+      <c r="B62" t="s">
+        <v>318</v>
+      </c>
+      <c r="C62" t="s">
+        <v>308</v>
+      </c>
+      <c r="D62" t="s">
+        <v>319</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>321</v>
+      </c>
+      <c r="C63" t="s">
+        <v>268</v>
+      </c>
+      <c r="D63" t="s">
+        <v>322</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>323</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2549,32 +4141,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -2602,7 +4194,7 @@
         <v>43251</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2610,7 +4202,7 @@
         <v>43251</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added documents with more info
</commit_message>
<xml_diff>
--- a/docs/Metrics.xlsx
+++ b/docs/Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr backupFile="1"/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13095"/>
+    <workbookView windowWidth="28695" windowHeight="13095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Discoveries" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353">
   <si>
     <t>Discovery ID</t>
   </si>
@@ -511,6 +511,15 @@
     <t>discover.ext_http_verbs</t>
   </si>
   <si>
+    <t>Top n rarely downloaded files (hash)</t>
+  </si>
+  <si>
+    <t>FILE_HASH</t>
+  </si>
+  <si>
+    <t>discover.downloaded_files</t>
+  </si>
+  <si>
     <t>Metric</t>
   </si>
   <si>
@@ -529,6 +538,9 @@
     <t>smart-onion.metrics.reconnaissance.pings_from_ext_ip.xxx.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>pings_from_host</t>
+  </si>
+  <si>
     <t>Number of SYN packets from EXT_IP to DMZ or LAN IPs</t>
   </si>
   <si>
@@ -538,6 +550,9 @@
     <t>smart-onion.metrics.reconnaissance.syn_from_ext_ip.xxx.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>orphan_syn_messages_from_host</t>
+  </si>
+  <si>
     <t>Number of FIN packets from EXT_IP to DMZ or LAN IPs</t>
   </si>
   <si>
@@ -565,27 +580,42 @@
     <t>smart-onion.metrics.reconnaissance.ports_attempted_by_ext_ip.xxx.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>ports_used_by_host</t>
+  </si>
+  <si>
     <t>Hash of sorted list of unique ports on which EXT_IP attempted to connect to the network</t>
   </si>
   <si>
     <t>smart-onion.metrics.reconnaissance.ports_list_attempted_by_ext_ip.xxx.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>ports_used_by_host_list_hash</t>
+  </si>
+  <si>
     <t>Number of pings from external IPs to PUB_IP</t>
   </si>
   <si>
     <t>smart-onion.metrics.reconnaissance.pings_to_pub_ip.xxx.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>pings_to_pub_ip</t>
+  </si>
+  <si>
     <t>Number of ports in which connections were attempted from external IPs to PUB_IP</t>
   </si>
   <si>
     <t>smart-onion.metrics.reconnaissance.ports_attempted_to_pub_ip.xxx.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>ports_used_to_host</t>
+  </si>
+  <si>
     <t>smart-onion.metrics.reconnaissance.ports_list_attempted_to_pub_ip.xxx.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>ports_used_to_host_list_hash</t>
+  </si>
+  <si>
     <t>Number of FIN packets from PUB_IP (to ext IP)</t>
   </si>
   <si>
@@ -607,12 +637,18 @@
     <t>smart-onion.metrics.reconnaissance.dns_tcp_requests_in_10mins</t>
   </si>
   <si>
+    <t>dns_tcp_requests</t>
+  </si>
+  <si>
     <t>Number of DNS queries in 10 mins per DNS_IP</t>
   </si>
   <si>
     <t>smart-onion.metrics.network.general_health.dns_queries_to_ip.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>dns_queries_to_ip</t>
+  </si>
+  <si>
     <t>Number of DNS queries in 10 mins that resulted in NXDOMAIN per DNS_IP</t>
   </si>
   <si>
@@ -622,12 +658,18 @@
     <t>smart-onion.metrics.dga.number_of_dns_queries_responded_with_nxdmomain_per_server.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>dns_nxdomain_queries_to_ip</t>
+  </si>
+  <si>
     <t>Number of DNS queries in 10 mins that resulted in NXDOMAIN per LAN_IP</t>
   </si>
   <si>
     <t>smart-onion.metrics.dga.number_of_dns_queries_responded_with_nxdmomain_per_client.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>dns_nxdomain_queries_from_ip</t>
+  </si>
+  <si>
     <t>Number of clients who sent queries with the DNS_QRY_FLAG flag in 10 mins</t>
   </si>
   <si>
@@ -637,6 +679,9 @@
     <t>smart-onion.metrics.reconnaissance.dns_interrogation.number_of_clients_per_dns_qry_flag.xxxx</t>
   </si>
   <si>
+    <t>number_of_clients_per_dns_qry_flag</t>
+  </si>
+  <si>
     <t>Files downloaded from TFTP_SRV_IP in the past 10 mins</t>
   </si>
   <si>
@@ -646,13 +691,19 @@
     <t>smart-onion.metrics.reconnaissance.files_downloaded_from_tftp_server.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>Need to test this to find out who that would appear in the log</t>
+  </si>
+  <si>
     <t>Number of requests per HTTP_VERB per WebServer</t>
   </si>
   <si>
     <t>Reconnaissance/HTTP</t>
   </si>
   <si>
-    <t>smart-onion.metrics.reconnaissance.verbs_per_webserver.xxx.xxx.xxx.xxx</t>
+    <t>smart-onion.metrics.reconnaissance.requests_per_webserver_per_verb.xxx.xxx.xxx.xxx.mmmm</t>
+  </si>
+  <si>
+    <t>number_of_requests_per_verb_per_website</t>
   </si>
   <si>
     <t>Number of connections per DPORT</t>
@@ -664,6 +715,9 @@
     <t>smart-onion.metrics.wierd_behaviour.number_of_connections_to_port.nnnnn</t>
   </si>
   <si>
+    <t>number_of_connections_to_port</t>
+  </si>
+  <si>
     <t>Number of connections to a null SMB session on WORKSTATION_IP</t>
   </si>
   <si>
@@ -688,6 +742,9 @@
     <t>smart-onion.metrics.phishing.highest_similarity_to_any_top_searched_fqdn.xxxxx.xxxxx.xxxxx</t>
   </si>
   <si>
+    <t>highest_similarity_to_any_top_searched_fqdn</t>
+  </si>
+  <si>
     <t>Number of connections to the workstations segments initiated by SERVER_IP</t>
   </si>
   <si>
@@ -989,6 +1046,12 @@
   </si>
   <si>
     <t>events_per_day</t>
+  </si>
+  <si>
+    <t>Number of unique source IPs that requested file FILE_HASH</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.malicious_file_download.hhhhhhhhhh</t>
   </si>
   <si>
     <t>Workstations</t>
@@ -1020,12 +1083,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1041,13 +1104,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -1057,10 +1113,41 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1078,90 +1165,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1177,6 +1181,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -1184,9 +1196,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1207,7 +1263,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1219,31 +1347,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1261,7 +1419,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1273,115 +1431,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1410,11 +1466,61 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1442,232 +1548,176 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1987,8 +2037,8 @@
   <sheetPr/>
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -1997,7 +2047,7 @@
     <col min="2" max="2" width="100.428571428571" customWidth="1"/>
     <col min="3" max="3" width="22.8571428571429" customWidth="1"/>
     <col min="4" max="4" width="73.2857142857143" customWidth="1"/>
-    <col min="5" max="5" width="23.2857142857143" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.2857142857143" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2013,7 +2063,7 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -2033,7 +2083,7 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2050,7 +2100,7 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2067,7 +2117,7 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
@@ -2087,7 +2137,7 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">
@@ -2107,7 +2157,7 @@
       <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2124,7 +2174,7 @@
       <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2141,7 +2191,7 @@
       <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2158,7 +2208,7 @@
       <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2175,7 +2225,7 @@
       <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2192,7 +2242,7 @@
       <c r="D11" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2209,7 +2259,7 @@
       <c r="D12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2226,7 +2276,7 @@
       <c r="D13" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2243,7 +2293,7 @@
       <c r="D14" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2260,7 +2310,7 @@
       <c r="D15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2277,7 +2327,7 @@
       <c r="D16" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2291,7 +2341,7 @@
       <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F17" t="s">
@@ -2308,7 +2358,7 @@
       <c r="C18" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F18" t="s">
@@ -2325,7 +2375,7 @@
       <c r="C19" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F19" t="s">
@@ -2345,7 +2395,7 @@
       <c r="D20" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2362,7 +2412,7 @@
       <c r="D21" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2379,7 +2429,7 @@
       <c r="D22" t="s">
         <v>64</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2393,7 +2443,7 @@
       <c r="C23" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F23" t="s">
@@ -2410,7 +2460,7 @@
       <c r="C24" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F24" t="s">
@@ -2427,7 +2477,7 @@
       <c r="C25" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F25" t="s">
@@ -2447,7 +2497,7 @@
       <c r="D26" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2464,7 +2514,7 @@
       <c r="D27" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2481,7 +2531,7 @@
       <c r="D28" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2495,7 +2545,7 @@
       <c r="C29" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F29" t="s">
@@ -2512,7 +2562,7 @@
       <c r="C30" t="s">
         <v>82</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F30" t="s">
@@ -2532,7 +2582,7 @@
       <c r="D31" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2549,7 +2599,7 @@
       <c r="D32" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2563,10 +2613,10 @@
       <c r="C33" t="s">
         <v>90</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2583,7 +2633,7 @@
       <c r="D34" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2597,10 +2647,10 @@
       <c r="C35" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F35" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2617,7 +2667,7 @@
       <c r="D36" t="s">
         <v>98</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2634,7 +2684,7 @@
       <c r="D37" t="s">
         <v>101</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2648,10 +2698,10 @@
       <c r="C38" t="s">
         <v>103</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2665,10 +2715,10 @@
       <c r="C39" t="s">
         <v>106</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2682,10 +2732,10 @@
       <c r="C40" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2702,7 +2752,7 @@
       <c r="D41" t="s">
         <v>113</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2719,7 +2769,7 @@
       <c r="D42" t="s">
         <v>115</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2736,7 +2786,7 @@
       <c r="D43" t="s">
         <v>118</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2753,7 +2803,7 @@
       <c r="D44" t="s">
         <v>120</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2770,7 +2820,7 @@
       <c r="D45" t="s">
         <v>123</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2787,7 +2837,7 @@
       <c r="D46" t="s">
         <v>125</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2804,7 +2854,7 @@
       <c r="D47" t="s">
         <v>128</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2821,7 +2871,7 @@
       <c r="D48" t="s">
         <v>130</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2838,7 +2888,7 @@
       <c r="D49" t="s">
         <v>133</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2855,7 +2905,7 @@
       <c r="D50" t="s">
         <v>135</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2872,7 +2922,7 @@
       <c r="D51" t="s">
         <v>137</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2889,7 +2939,7 @@
       <c r="D52" t="s">
         <v>140</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2906,7 +2956,7 @@
       <c r="D53" t="s">
         <v>143</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2923,7 +2973,7 @@
       <c r="D54" t="s">
         <v>146</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2940,7 +2990,7 @@
       <c r="D55" t="s">
         <v>149</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2957,7 +3007,7 @@
       <c r="D56" t="s">
         <v>152</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2974,7 +3024,7 @@
       <c r="D57" t="s">
         <v>155</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2991,7 +3041,7 @@
       <c r="D58" t="s">
         <v>158</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="2">
         <v>2</v>
       </c>
     </row>
@@ -3008,7 +3058,7 @@
       <c r="D59" t="s">
         <v>161</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="2">
         <v>2</v>
       </c>
     </row>
@@ -3025,13 +3075,25 @@
       <c r="D60" t="s">
         <v>163</v>
       </c>
-      <c r="E60" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="E60" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>164</v>
+      </c>
+      <c r="C61" t="s">
+        <v>165</v>
+      </c>
+      <c r="D61" t="s">
+        <v>166</v>
+      </c>
+      <c r="E61" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:1">
@@ -3164,13 +3226,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="12.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="132.428571428571" customWidth="1"/>
@@ -3179,147 +3241,207 @@
     <col min="5" max="5" width="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>169</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>172</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>176</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>180</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>183</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>186</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>189</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>192</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C9" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D9" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>195</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C10" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s">
-        <v>188</v>
+        <v>197</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3327,13 +3449,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C11" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D11" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3341,223 +3463,310 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="C12" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="C13" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>205</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C14" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="D14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>208</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="C15" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="D15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>212</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="C16" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>215</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="C17" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>219</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="C18" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="D18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>223</v>
+      </c>
+      <c r="G18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="19" ht="13" customHeight="1" spans="1:6">
       <c r="A19">
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="C19" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="D19" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>227</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="C20" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="D20" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>231</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="C21" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="D21" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>231</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="C22" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="D22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>231</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="C23" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="D23" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>231</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="C24" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="D24" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>235</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="C25" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="D25" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>235</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="C26" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="D26" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>235</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="C27" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="D27" t="s">
-        <v>222</v>
+        <v>240</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3565,13 +3774,13 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="C28" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D28" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3579,13 +3788,13 @@
         <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="C29" t="s">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="D29" t="s">
-        <v>228</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3593,13 +3802,13 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
       <c r="C30" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="D30" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3607,13 +3816,13 @@
         <v>21</v>
       </c>
       <c r="B31" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="C31" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="D31" t="s">
-        <v>233</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3621,13 +3830,13 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="C32" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="D32" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3635,13 +3844,13 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="C33" t="s">
-        <v>238</v>
+        <v>257</v>
       </c>
       <c r="D33" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3649,13 +3858,13 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="C34" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="D34" t="s">
-        <v>236</v>
+        <v>255</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3663,13 +3872,13 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="C35" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="D35" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3677,13 +3886,13 @@
         <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>243</v>
+        <v>262</v>
       </c>
       <c r="C36" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="D36" t="s">
-        <v>244</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3691,13 +3900,13 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>245</v>
+        <v>264</v>
       </c>
       <c r="C37" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="D37" t="s">
-        <v>246</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3705,13 +3914,13 @@
         <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="C38" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="D38" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3719,13 +3928,13 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="C39" t="s">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="D39" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3733,13 +3942,13 @@
         <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="C40" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="D40" t="s">
-        <v>255</v>
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3747,13 +3956,13 @@
         <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="C41" t="s">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="D41" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3761,13 +3970,13 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="C42" t="s">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="D42" t="s">
-        <v>260</v>
+        <v>279</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3775,13 +3984,13 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="C43" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D43" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3789,13 +3998,13 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="C44" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D44" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3803,319 +4012,411 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
       <c r="C45" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="D45" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
       <c r="C46" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="D46" t="s">
-        <v>269</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>288</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>271</v>
+        <v>290</v>
       </c>
       <c r="C47" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="D47" t="s">
-        <v>273</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>292</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="C48" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="D48" t="s">
-        <v>277</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>296</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="C49" t="s">
-        <v>276</v>
+        <v>295</v>
       </c>
       <c r="D49" t="s">
-        <v>280</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>299</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
       <c r="C50" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D50" t="s">
-        <v>283</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>302</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
       <c r="C51" t="s">
-        <v>286</v>
+        <v>305</v>
       </c>
       <c r="D51" t="s">
-        <v>287</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>306</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="C52" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="D52" t="s">
-        <v>291</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>310</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="C53" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="D53" t="s">
-        <v>294</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>313</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="C54" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="D54" t="s">
-        <v>297</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>316</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="C55" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="D55" t="s">
-        <v>297</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>316</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="F55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="C56" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="D56" t="s">
-        <v>301</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>320</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="C57" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="D57" t="s">
-        <v>301</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>320</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
       <c r="C58" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="D58" t="s">
-        <v>305</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>324</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>307</v>
+        <v>326</v>
       </c>
       <c r="C59" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="D59" t="s">
-        <v>309</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>328</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60">
         <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
       <c r="C60" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="D60" t="s">
-        <v>312</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>331</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61">
         <v>34</v>
       </c>
       <c r="B61" t="s">
-        <v>314</v>
+        <v>333</v>
       </c>
       <c r="C61" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="D61" t="s">
-        <v>316</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>335</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62">
         <v>25</v>
       </c>
       <c r="B62" t="s">
-        <v>318</v>
+        <v>337</v>
       </c>
       <c r="C62" t="s">
-        <v>308</v>
+        <v>327</v>
       </c>
       <c r="D62" t="s">
-        <v>319</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>338</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G62" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
       <c r="C63" t="s">
-        <v>268</v>
+        <v>287</v>
       </c>
       <c r="D63" t="s">
-        <v>322</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>323</v>
+        <v>341</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>343</v>
+      </c>
+      <c r="C64" t="s">
+        <v>327</v>
+      </c>
+      <c r="D64" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -4141,32 +4442,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>324</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>325</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>326</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>327</v>
+        <v>348</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>328</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>329</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -4194,7 +4495,7 @@
         <v>43251</v>
       </c>
       <c r="B1" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4202,7 +4503,7 @@
         <v>43251</v>
       </c>
       <c r="B2" t="s">
-        <v>331</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Redesigned the directory structure
</commit_message>
<xml_diff>
--- a/docs/Metrics.xlsx
+++ b/docs/Metrics.xlsx
@@ -12,12 +12,15 @@
     <sheet name="IP Ranges" sheetId="3" r:id="rId3"/>
     <sheet name="Ideas" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Metrics!$A$1:$G$66</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365">
   <si>
     <t>Discovery ID</t>
   </si>
@@ -754,6 +757,9 @@
     <t>smart-onion.metrics.lateral_movement.number_of_connections_to_workstations_for_server.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>number_of_connections_to_workstations_for_server</t>
+  </si>
+  <si>
     <t>Number of unique organization IP addresses that connected to EXT_IP in last week</t>
   </si>
   <si>
@@ -763,6 +769,9 @@
     <t>smart-onion.metrics.command_and_control.number_of_internal_ips_connected_to_ext_ip.xxx.xxx.xxx.xxx</t>
   </si>
   <si>
+    <t>number_of_connections_to_ext_ip</t>
+  </si>
+  <si>
     <t>Number of unique organization IP addresses that connected to websites identified by certificates signed by CERT_ISSUER in last week</t>
   </si>
   <si>
@@ -772,12 +781,18 @@
     <t>smart-onion.metrics.phishing.number_of_internal_ips_connected_to_sites_signed_by_issuer.aaaa</t>
   </si>
   <si>
+    <t>number_of_internal_ips_connected_to_sites_signed_by_issuer</t>
+  </si>
+  <si>
     <t>Number of unique organization IP addresses that connected to websites identified by the certificate CERT_CN in last week</t>
   </si>
   <si>
     <t>smart-onion.metrics.phishing.number_of_internal_ips_connected_to_sites_signed_by_cert_cn.aaaa</t>
   </si>
   <si>
+    <t>number_of_internal_ips_connected_to_sites_signed_by_cert_cn</t>
+  </si>
+  <si>
     <t>Length of DNS_REC</t>
   </si>
   <si>
@@ -787,6 +802,9 @@
     <t>smart-onion.metrics.phishing.dns_record_length.xxxxx.xxxxx.xxxxx</t>
   </si>
   <si>
+    <t>get-length or get-length_b64</t>
+  </si>
+  <si>
     <t>Highest similarity of MAIL_ADDR to any of the top n most frequently used mail senders (from outside the organization)</t>
   </si>
   <si>
@@ -835,6 +853,9 @@
     <t>smart-onion.metrics.web_reqs.number_of_web_reqs_per_url.aaaa.aaaa</t>
   </si>
   <si>
+    <t>number_of_requests_per_url</t>
+  </si>
+  <si>
     <t>Hash of WEB_FILE</t>
   </si>
   <si>
@@ -859,6 +880,9 @@
     <t>smart-onion.data.new_host.known_hosts_list</t>
   </si>
   <si>
+    <t>Needs a relational database to achieve that</t>
+  </si>
+  <si>
     <t>Number of connections via SMBv1 to WORKSTATION_IP</t>
   </si>
   <si>
@@ -1052,6 +1076,21 @@
   </si>
   <si>
     <t>smart-onion.metrics.malicious_file_download.hhhhhhhhhh</t>
+  </si>
+  <si>
+    <t>smart-onion.metrics.phishing.highest_similarity_to_any_top_virtual_host.xxxxx.xxxxx.xxxxx</t>
+  </si>
+  <si>
+    <t>highest_similarity_to_any_top_searched_virtual_host</t>
+  </si>
+  <si>
+    <t>Certificate issuer per website</t>
+  </si>
+  <si>
+    <t>smart-onion.data.certificate_issuer_per_virtual_host.xxxxxxxx</t>
+  </si>
+  <si>
+    <t>certificate_issuer_per_virtual_host</t>
   </si>
   <si>
     <t>Workstations</t>
@@ -1083,10 +1122,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1113,8 +1152,31 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1128,31 +1190,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1174,10 +1213,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1190,7 +1229,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1203,23 +1242,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1233,18 +1272,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1263,19 +1302,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1293,7 +1332,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1305,7 +1428,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1317,127 +1470,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1466,17 +1505,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1501,6 +1534,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1539,96 +1587,87 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1637,55 +1676,55 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1719,6 +1758,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3226,10 +3268,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="6"/>
@@ -3762,14 +3804,14 @@
       <c r="D27" t="s">
         <v>240</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="3" t="s">
         <v>241</v>
       </c>
       <c r="F27">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>8</v>
       </c>
@@ -3782,61 +3824,88 @@
       <c r="D28" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C29" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D29" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>248</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C30" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D30" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>252</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>21</v>
       </c>
       <c r="B31" t="s">
+        <v>254</v>
+      </c>
+      <c r="C31" t="s">
         <v>251</v>
       </c>
-      <c r="C31" t="s">
-        <v>249</v>
-      </c>
       <c r="D31" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>255</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C32" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D32" t="s">
-        <v>255</v>
+        <v>259</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3844,27 +3913,33 @@
         <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C33" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D33" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C34" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="D34" t="s">
-        <v>255</v>
+        <v>259</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3872,13 +3947,13 @@
         <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C35" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D35" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3886,13 +3961,13 @@
         <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="C36" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D36" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3900,13 +3975,13 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="C37" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="D37" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3914,27 +3989,33 @@
         <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="C38" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="D38" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="C39" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="D39" t="s">
-        <v>271</v>
+        <v>276</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3942,13 +4023,13 @@
         <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C40" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="D40" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3956,27 +4037,33 @@
         <v>28</v>
       </c>
       <c r="B41" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C41" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="D41" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C42" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="D42" t="s">
-        <v>279</v>
+        <v>285</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3984,13 +4071,13 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="C43" t="s">
         <v>243</v>
       </c>
       <c r="D43" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3998,13 +4085,13 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="C44" t="s">
         <v>243</v>
       </c>
       <c r="D44" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -4012,13 +4099,13 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="C45" t="s">
         <v>243</v>
       </c>
       <c r="D45" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -4026,16 +4113,16 @@
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="C46" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D46" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="F46">
         <v>2</v>
@@ -4046,16 +4133,16 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C47" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="D47" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>14</v>
@@ -4069,16 +4156,16 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="C48" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D48" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="F48">
         <v>2</v>
@@ -4089,16 +4176,16 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="C49" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D49" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="F49">
         <v>2</v>
@@ -4109,16 +4196,16 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="C50" t="s">
         <v>185</v>
       </c>
       <c r="D50" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>14</v>
@@ -4132,16 +4219,16 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="C51" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D51" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>14</v>
@@ -4155,16 +4242,16 @@
         <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="C52" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D52" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>14</v>
@@ -4178,16 +4265,16 @@
         <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="C53" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D53" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="F53">
         <v>2</v>
@@ -4198,16 +4285,16 @@
         <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="C54" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D54" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="F54">
         <v>2</v>
@@ -4218,16 +4305,16 @@
         <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="C55" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D55" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="F55">
         <v>2</v>
@@ -4238,16 +4325,16 @@
         <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="C56" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D56" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F56">
         <v>2</v>
@@ -4258,16 +4345,16 @@
         <v>19</v>
       </c>
       <c r="B57" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="C57" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D57" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="F57">
         <v>2</v>
@@ -4278,16 +4365,16 @@
         <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="C58" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D58" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="F58">
         <v>2</v>
@@ -4298,16 +4385,16 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="C59" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="D59" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>14</v>
@@ -4321,16 +4408,16 @@
         <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="C60" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="D60" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>14</v>
@@ -4344,16 +4431,16 @@
         <v>34</v>
       </c>
       <c r="B61" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="C61" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="D61" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="F61" s="6" t="s">
         <v>14</v>
@@ -4367,16 +4454,16 @@
         <v>25</v>
       </c>
       <c r="B62" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="C62" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="D62" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>14</v>
@@ -4390,16 +4477,16 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="C63" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D63" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="F63">
         <v>2</v>
@@ -4410,16 +4497,54 @@
         <v>60</v>
       </c>
       <c r="B64" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="C64" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="D64" t="s">
-        <v>344</v>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="65" customFormat="1" spans="1:6">
+      <c r="A65">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>238</v>
+      </c>
+      <c r="C65" t="s">
+        <v>239</v>
+      </c>
+      <c r="D65" t="s">
+        <v>352</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66" t="s">
+        <v>354</v>
+      </c>
+      <c r="C66" t="s">
+        <v>239</v>
+      </c>
+      <c r="D66" t="s">
+        <v>355</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G66"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
@@ -4442,32 +4567,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>346</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>350</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -4495,7 +4620,7 @@
         <v>43251</v>
       </c>
       <c r="B1" t="s">
-        <v>351</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4503,7 +4628,7 @@
         <v>43251</v>
       </c>
       <c r="B2" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>